<commit_message>
Update regression analysis files: modify Progress document with detailed explanations on quasi-complete separation, adjust paths in ridge regression script, and refine control variable handling for improved model accuracy.
</commit_message>
<xml_diff>
--- a/Good one/3. Regression/GFDD.SI.01_3.3_regression_z-score_ridge.xlsx
+++ b/Good one/3. Regression/GFDD.SI.01_3.3_regression_z-score_ridge.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\creditriskbachelor\Good one\3. Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Licenta\work\creditriskbachelor\Good one\3. Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04845910-8BD4-4184-BE12-026E15F7B7F9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11928"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
     <sheet name="Regression" sheetId="2" r:id="rId2"/>
     <sheet name="Alpha_selection" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabele" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="231">
   <si>
     <t>Split</t>
   </si>
@@ -553,13 +553,358 @@
   </si>
   <si>
     <t>val_auc</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Train: The model distinguishes crisis from no-crisis better than random (0.5), but with moderate discrimination.</t>
+  </si>
+  <si>
+    <t>Validation: Similar to training, indicating consistent generalization</t>
+  </si>
+  <si>
+    <t>AUC = 0.66–0.68 means the model ranks higher-risk observations above lower-risk ones about 66–68% of the time.</t>
+  </si>
+  <si>
+    <t>For financial crisis prediction, this is modest but reasonable given the rarity of crises and the complexity of the task.</t>
+  </si>
+  <si>
+    <t>Train: Moderate prediction error. Lower is better (perfect = 0).</t>
+  </si>
+  <si>
+    <t>Validation: Slightly lower than training, which is a positive sign.</t>
+  </si>
+  <si>
+    <t>Conclusions</t>
+  </si>
+  <si>
+    <t>Economic interpretation</t>
+  </si>
+  <si>
+    <t>The model captures some signal: AUC &gt; 0.5 indicates predictive value beyond chance.</t>
+  </si>
+  <si>
+    <t>Modest discrimination: AUC around 0.66–0.68 suggests the model is useful but not highly precise.</t>
+  </si>
+  <si>
+    <t>Validation during crisis period: The 2008-2010 period includes the global financial crisis, and the model maintains similar performance, which is encouraging.</t>
+  </si>
+  <si>
+    <t> The model can help rank countries by risk, though it is not highly precise.</t>
+  </si>
+  <si>
+    <t>Limitations: AUC around 0.66–0.68 means the model misses many crises and may produce false alarms.</t>
+  </si>
+  <si>
+    <t>Comparison with unregularized model</t>
+  </si>
+  <si>
+    <t>Ridge reduced overfitting: Validation AUC improved from 0.515 (near random) to 0.660.</t>
+  </si>
+  <si>
+    <t>Validation log-loss improved dramatically: from 16.65 to 0.658.</t>
+  </si>
+  <si>
+    <t>Coefficients are now stable and interpretable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>No overfitting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Validation performance is similar to or slightly better than training, suggesting good generalization.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Consistent performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>: The model performs similarly on the 2008-2010 period (financial crisis) as on training.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ridge regularization appears effective</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>: The penalty helped avoid the extreme coefficients seen in the unregularized model.</t>
+    </r>
+  </si>
+  <si>
+    <t>Negative coefficient: higher lagged Z-Score is associated with lower crisis probability.</t>
+  </si>
+  <si>
+    <t>For a 1 standard deviation increase in lagged Z-Score, the log-odds of crisis decrease by 0.319.</t>
+  </si>
+  <si>
+    <t>The effect is moderate and economically meaningful.</t>
+  </si>
+  <si>
+    <t>Z-Score is a useful early warning indicator.</t>
+  </si>
+  <si>
+    <t>Economic meaning</t>
+  </si>
+  <si>
+    <t>Country fixed effects</t>
+  </si>
+  <si>
+    <t>Log-odds of crisis for the reference country (Afghanistan) in the reference year (1985)</t>
+  </si>
+  <si>
+    <t>Countries with positive coefficients have higher risk than Afghanistan</t>
+  </si>
+  <si>
+    <t>Year fixed effects</t>
+  </si>
+  <si>
+    <t>2001: higher baseline risk (recession, 9/11).</t>
+  </si>
+  <si>
+    <t>2002-2003: risk moderating but still above baseline.</t>
+  </si>
+  <si>
+    <t>2004-2006: lower baseline risk (expansion).</t>
+  </si>
+  <si>
+    <t>2006: lowest risk (pre-crisis peak).</t>
+  </si>
+  <si>
+    <t>2007: risk rising (early subprime signs), but still below baseline.</t>
+  </si>
+  <si>
+    <t>This pattern aligns with the economic cycle and the run-up to the 2008 crisis.</t>
+  </si>
+  <si>
+    <t>Each row represents one value of alpha_fe tried on train, evaluated on both train and validation</t>
+  </si>
+  <si>
+    <t>Performance when fitting with that alpha on the training data</t>
+  </si>
+  <si>
+    <t>Performance on the validation data (what really matters for choosing alpha)</t>
+  </si>
+  <si>
+    <r>
+      <t>As </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>alpha increases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, train performance gets worse (log-loss up, AUC down) but </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>validation performance improves</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Lower is better</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 0 is perfect</t>
+    </r>
+  </si>
+  <si>
+    <t>Here, a weighted log‑loss around 0.65–0.70 means the probabilities are reasonable but not perfect; the fact that train and validation log‑loss are similar means the model generalizes.</t>
+  </si>
+  <si>
+    <r>
+      <t>A measure of how close the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>predicted probabilities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> are to the true outcomes (0/1).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A measure of how well the model </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>ranks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> crisis vs non‑crisis cases, using the predicted probabilities</t>
+    </r>
+  </si>
+  <si>
+    <t>Log loss</t>
+  </si>
+  <si>
+    <t>It heavily penalizes “confident but wrong” predictions</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <r>
+      <t>Probabilistic meaning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>: AUC is the probability that a randomly chosen crisis observation gets a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>higher predicted risk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t> than a randomly chosen non‑crisis observation.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scale / interpretation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>1.0 = perfect ranking.</t>
+  </si>
+  <si>
+    <t>0.6–0.7 = modest / fair discrimination; 0.7–0.8 = good; &gt;0.8 = very good.</t>
+  </si>
+  <si>
+    <t>0.5 = random guessing </t>
+  </si>
+  <si>
+    <t>AUC ≈ 0.66–0.68 means the model correctly ranks a crisis above a non‑crisis about 66–68% of the time—useful, but not extremely strong discrimination.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,16 +917,93 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -604,14 +1026,429 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -628,6 +1465,173 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15239</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>146879</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagine 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="632461"/>
+          <a:ext cx="6743699" cy="4825558"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>58713</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagine 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3870960" y="38100"/>
+          <a:ext cx="4069080" cy="3495333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>15241</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>48912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagine 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="2567940"/>
+          <a:ext cx="4442460" cy="780432"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>32685</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>45721</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagine 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4991100" y="510541"/>
+          <a:ext cx="3736005" cy="3383280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -914,64 +1918,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="51.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>0.67535735503981376</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>0.67798890196737505</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>0.65804999875814707</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>0.66025641025641157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="76"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -979,7 +2005,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -990,7 +2016,7 @@
         <v>0.99833634187985554</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1001,7 +2027,7 @@
         <v>0.72668275049665287</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +2038,7 @@
         <v>0.99981669444348642</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +2049,7 @@
         <v>0.99979238018634486</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1034,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1045,7 +2071,7 @@
         <v>0.99982112854520722</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1056,7 +2082,7 @@
         <v>0.99982852138955858</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1067,7 +2093,7 @@
         <v>1.0030726265004279</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1078,7 +2104,7 @@
         <v>0.99981385160199898</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1089,7 +2115,7 @@
         <v>0.99983208889586528</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1100,7 +2126,7 @@
         <v>0.99983000621614937</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +2137,7 @@
         <v>0.99978485626611846</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1122,7 +2148,7 @@
         <v>0.99980794061141343</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1133,7 +2159,7 @@
         <v>0.99978615537807791</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1144,7 +2170,7 @@
         <v>0.99980785654521442</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +2181,7 @@
         <v>0.99997366506922958</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1166,7 +2192,7 @@
         <v>0.99986049957701928</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1177,7 +2203,7 @@
         <v>0.9997893949275205</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1188,7 +2214,7 @@
         <v>0.9998243052253607</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +2225,7 @@
         <v>0.99980985972919045</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1210,7 +2236,7 @@
         <v>0.99980959735423081</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +2247,7 @@
         <v>0.99981459746289114</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1232,7 +2258,7 @@
         <v>0.99978718900810792</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1243,7 +2269,7 @@
         <v>0.99981722607211643</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1254,7 +2280,7 @@
         <v>0.99979312609702697</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1265,7 +2291,7 @@
         <v>0.99979317949708557</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -1276,7 +2302,7 @@
         <v>0.99980637648055426</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -1287,7 +2313,7 @@
         <v>0.99989290461629499</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1298,7 +2324,7 @@
         <v>0.99979571481439711</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1309,7 +2335,7 @@
         <v>0.99981881271410933</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +2346,7 @@
         <v>0.99983672857055905</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1331,7 +2357,7 @@
         <v>0.99986285049153945</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +2368,7 @@
         <v>0.99979214976703767</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1353,7 +2379,7 @@
         <v>0.99980412654119333</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +2390,7 @@
         <v>0.99980600954307419</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +2401,7 @@
         <v>0.99982372769392636</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +2412,7 @@
         <v>0.99982961581170693</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1397,7 +2423,7 @@
         <v>0.99982927736918981</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1408,7 +2434,7 @@
         <v>0.99977878613652793</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1419,7 +2445,7 @@
         <v>0.99980402914863264</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1430,7 +2456,7 @@
         <v>0.99983079268672104</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1441,7 +2467,7 @@
         <v>0.99978576018334642</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -1452,7 +2478,7 @@
         <v>0.99979168056089318</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1463,7 +2489,7 @@
         <v>0.99982265018306915</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1474,7 +2500,7 @@
         <v>1.0034411702812831</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -1485,7 +2511,7 @@
         <v>1.002119367498167</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -1496,7 +2522,7 @@
         <v>0.99980798347564392</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -1507,7 +2533,7 @@
         <v>0.99982181163122896</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
@@ -1518,7 +2544,7 @@
         <v>0.9997938415700296</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
@@ -1529,7 +2555,7 @@
         <v>0.99984939419622743</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
@@ -1540,7 +2566,7 @@
         <v>0.99979274566720222</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
@@ -1551,7 +2577,7 @@
         <v>0.99981795947338215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -1562,7 +2588,7 @@
         <v>0.99982573403351727</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -1573,7 +2599,7 @@
         <v>0.99989007636774863</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
@@ -1584,7 +2610,7 @@
         <v>0.99991846787716743</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -1595,7 +2621,7 @@
         <v>0.99980055555842162</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
@@ -1606,7 +2632,7 @@
         <v>0.9998013257666245</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>64</v>
       </c>
@@ -1617,7 +2643,7 @@
         <v>0.99994378284634156</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1628,7 +2654,7 @@
         <v>0.99990465393434969</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
@@ -1639,7 +2665,7 @@
         <v>0.99985135207870302</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -1650,7 +2676,7 @@
         <v>0.99981465510776391</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>68</v>
       </c>
@@ -1661,7 +2687,7 @@
         <v>0.99987955275759322</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>69</v>
       </c>
@@ -1672,7 +2698,7 @@
         <v>0.99986131404923295</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>70</v>
       </c>
@@ -1683,7 +2709,7 @@
         <v>0.99983601773109976</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
@@ -1694,7 +2720,7 @@
         <v>0.99978525292142706</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -1705,7 +2731,7 @@
         <v>0.99996676358911507</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
@@ -1716,7 +2742,7 @@
         <v>0.99980561254019795</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -1727,7 +2753,7 @@
         <v>1.000792968847632</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>75</v>
       </c>
@@ -1738,7 +2764,7 @@
         <v>0.99994694788111349</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>76</v>
       </c>
@@ -1749,7 +2775,7 @@
         <v>0.99980828716651293</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>77</v>
       </c>
@@ -1760,7 +2786,7 @@
         <v>0.99985099162984525</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>78</v>
       </c>
@@ -1771,7 +2797,7 @@
         <v>0.99981497413249509</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
@@ -1782,7 +2808,7 @@
         <v>0.99986624092371723</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>80</v>
       </c>
@@ -1793,7 +2819,7 @@
         <v>1.001138475856352</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>81</v>
       </c>
@@ -1804,7 +2830,7 @@
         <v>0.99988011095799867</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>82</v>
       </c>
@@ -1815,7 +2841,7 @@
         <v>0.99977034217910377</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>83</v>
       </c>
@@ -1826,7 +2852,7 @@
         <v>0.99981800141534449</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
@@ -1837,7 +2863,7 @@
         <v>0.99996924236889628</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>85</v>
       </c>
@@ -1848,7 +2874,7 @@
         <v>0.99981545324986298</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>86</v>
       </c>
@@ -1859,7 +2885,7 @@
         <v>0.99982992431142281</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>87</v>
       </c>
@@ -1870,7 +2896,7 @@
         <v>0.99978059411047104</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>88</v>
       </c>
@@ -1881,7 +2907,7 @@
         <v>0.99981254283525256</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>89</v>
       </c>
@@ -1892,7 +2918,7 @@
         <v>0.99989304714612559</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>90</v>
       </c>
@@ -1903,7 +2929,7 @@
         <v>0.99985698917879029</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>91</v>
       </c>
@@ -1914,7 +2940,7 @@
         <v>0.99978212538237399</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>92</v>
       </c>
@@ -1925,7 +2951,7 @@
         <v>0.99985666699046849</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>93</v>
       </c>
@@ -1936,7 +2962,7 @@
         <v>0.99988749786530595</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>94</v>
       </c>
@@ -1947,7 +2973,7 @@
         <v>0.99981024820046849</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>95</v>
       </c>
@@ -1958,7 +2984,7 @@
         <v>0.99981261266298471</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>96</v>
       </c>
@@ -1969,7 +2995,7 @@
         <v>0.99981191897821398</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>97</v>
       </c>
@@ -1980,7 +3006,7 @@
         <v>0.99981913478527051</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>98</v>
       </c>
@@ -1991,7 +3017,7 @@
         <v>0.99984443574859561</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>99</v>
       </c>
@@ -2002,7 +3028,7 @@
         <v>0.99985552441575409</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>100</v>
       </c>
@@ -2013,7 +3039,7 @@
         <v>0.9998364686856307</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>101</v>
       </c>
@@ -2024,7 +3050,7 @@
         <v>0.99983110861094027</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>102</v>
       </c>
@@ -2035,7 +3061,7 @@
         <v>0.99980048434496249</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>103</v>
       </c>
@@ -2046,7 +3072,7 @@
         <v>0.99997001242172845</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>104</v>
       </c>
@@ -2057,7 +3083,7 @@
         <v>0.99987277040848044</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>105</v>
       </c>
@@ -2068,7 +3094,7 @@
         <v>0.99988664729309851</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>106</v>
       </c>
@@ -2079,7 +3105,7 @@
         <v>0.99988113732587269</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>107</v>
       </c>
@@ -2090,7 +3116,7 @@
         <v>0.99987340500111033</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>108</v>
       </c>
@@ -2101,7 +3127,7 @@
         <v>0.99993371929113228</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>109</v>
       </c>
@@ -2112,7 +3138,7 @@
         <v>0.99995956850993872</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>110</v>
       </c>
@@ -2123,7 +3149,7 @@
         <v>0.99983401958576079</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>111</v>
       </c>
@@ -2134,7 +3160,7 @@
         <v>0.99982055989019236</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>112</v>
       </c>
@@ -2145,7 +3171,7 @@
         <v>0.99998143425977393</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>113</v>
       </c>
@@ -2156,7 +3182,7 @@
         <v>1.0010840624113211</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>114</v>
       </c>
@@ -2167,7 +3193,7 @@
         <v>0.99980816295647246</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>115</v>
       </c>
@@ -2178,7 +3204,7 @@
         <v>0.99981141493609194</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>116</v>
       </c>
@@ -2189,7 +3215,7 @@
         <v>0.99980642264635022</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>117</v>
       </c>
@@ -2200,7 +3226,7 @@
         <v>0.99978751805164057</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>118</v>
       </c>
@@ -2211,7 +3237,7 @@
         <v>0.99981876514706869</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>119</v>
       </c>
@@ -2222,7 +3248,7 @@
         <v>0.99979183954224982</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>120</v>
       </c>
@@ -2233,7 +3259,7 @@
         <v>0.9998884531792005</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>121</v>
       </c>
@@ -2244,7 +3270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>122</v>
       </c>
@@ -2255,7 +3281,7 @@
         <v>0.9998130275883822</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>123</v>
       </c>
@@ -2266,7 +3292,7 @@
         <v>0.99981409629726536</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>124</v>
       </c>
@@ -2277,7 +3303,7 @@
         <v>0.99987316295757578</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>125</v>
       </c>
@@ -2288,7 +3314,7 @@
         <v>0.99978638403259645</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>126</v>
       </c>
@@ -2299,7 +3325,7 @@
         <v>0.9997947100844542</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>127</v>
       </c>
@@ -2310,7 +3336,7 @@
         <v>0.99985419704463607</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>128</v>
       </c>
@@ -2321,7 +3347,7 @@
         <v>0.99980878214828794</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>129</v>
       </c>
@@ -2332,7 +3358,7 @@
         <v>0.99979496894889197</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>130</v>
       </c>
@@ -2343,7 +3369,7 @@
         <v>0.99982798548131624</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>131</v>
       </c>
@@ -2354,7 +3380,7 @@
         <v>0.99991415820535845</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>132</v>
       </c>
@@ -2365,7 +3391,7 @@
         <v>0.99981956438902453</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>133</v>
       </c>
@@ -2376,7 +3402,7 @@
         <v>0.99981019636997115</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>134</v>
       </c>
@@ -2387,7 +3413,7 @@
         <v>0.99980160199415335</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>135</v>
       </c>
@@ -2398,7 +3424,7 @@
         <v>0.99978610616513386</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>136</v>
       </c>
@@ -2409,7 +3435,7 @@
         <v>0.99985051172344686</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>137</v>
       </c>
@@ -2420,7 +3446,7 @@
         <v>1.002544252492612</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>138</v>
       </c>
@@ -2431,7 +3457,7 @@
         <v>0.99977343330956114</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>139</v>
       </c>
@@ -2442,7 +3468,7 @@
         <v>0.99986717337533293</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>140</v>
       </c>
@@ -2453,7 +3479,7 @@
         <v>0.99982454814262867</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>141</v>
       </c>
@@ -2464,7 +3490,7 @@
         <v>0.99984529811759748</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>142</v>
       </c>
@@ -2475,7 +3501,7 @@
         <v>0.99983556219845793</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>143</v>
       </c>
@@ -2486,7 +3512,7 @@
         <v>0.99979822438156329</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>144</v>
       </c>
@@ -2497,7 +3523,7 @@
         <v>0.99990153346600674</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>145</v>
       </c>
@@ -2508,7 +3534,7 @@
         <v>0.99984885835380255</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>146</v>
       </c>
@@ -2519,7 +3545,7 @@
         <v>0.99994370177461345</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>147</v>
       </c>
@@ -2530,7 +3556,7 @@
         <v>0.99991755710221042</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>148</v>
       </c>
@@ -2541,7 +3567,7 @@
         <v>0.9997758189549909</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>149</v>
       </c>
@@ -2552,7 +3578,7 @@
         <v>0.99994471265172002</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>150</v>
       </c>
@@ -2563,7 +3589,7 @@
         <v>0.99981492640287872</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>151</v>
       </c>
@@ -2574,7 +3600,7 @@
         <v>0.99987499233958732</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>152</v>
       </c>
@@ -2585,7 +3611,7 @@
         <v>1.0010906110612929</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>153</v>
       </c>
@@ -2596,7 +3622,7 @@
         <v>0.99979361336070138</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>154</v>
       </c>
@@ -2607,7 +3633,7 @@
         <v>0.99978217851161633</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>155</v>
       </c>
@@ -2618,7 +3644,7 @@
         <v>0.99985382870554684</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>156</v>
       </c>
@@ -2629,7 +3655,7 @@
         <v>1.000968810000451</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>157</v>
       </c>
@@ -2640,7 +3666,7 @@
         <v>1.0015754524597289</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>158</v>
       </c>
@@ -2651,7 +3677,7 @@
         <v>1.003955718621772</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>159</v>
       </c>
@@ -2662,7 +3688,7 @@
         <v>0.99981688095073207</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>160</v>
       </c>
@@ -2673,7 +3699,7 @@
         <v>0.99980327157857063</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>161</v>
       </c>
@@ -2684,7 +3710,7 @@
         <v>0.99979661036688405</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>162</v>
       </c>
@@ -2695,7 +3721,7 @@
         <v>0.99981407331655248</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>163</v>
       </c>
@@ -2706,7 +3732,7 @@
         <v>0.9997884664027068</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>164</v>
       </c>
@@ -2717,7 +3743,7 @@
         <v>0.99996877695468078</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>165</v>
       </c>
@@ -2728,7 +3754,7 @@
         <v>1.0051804569872571</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>166</v>
       </c>
@@ -2739,7 +3765,7 @@
         <v>1.0011388672645469</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>167</v>
       </c>
@@ -2750,7 +3776,7 @@
         <v>1.000530003661716</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>168</v>
       </c>
@@ -2761,7 +3787,7 @@
         <v>0.99913947945006831</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>169</v>
       </c>
@@ -2772,7 +3798,7 @@
         <v>0.99732335634664537</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>170</v>
       </c>
@@ -2783,7 +3809,7 @@
         <v>0.99611195139888797</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>171</v>
       </c>
@@ -2796,246 +3822,578 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>0.67535735503981376</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>0.67798890196737505</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>0.65804999875814707</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>0.66025641025641157</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="G2" s="41" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>3.511191734215128</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>0.67325389595975504</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>0.68421052631578605</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>0.65922575515668191</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>0.66012820512820636</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>1.2328467394420659</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>0.66741599761879511</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>0.7025951460119918</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>0.66261039666040533</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="7">
         <v>0.65952991452991583</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>0.43287612810830572</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>0.65191003070821651</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>0.74625861779048019</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>0.67229287902125012</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <v>0.65752136752136892</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>0.1519911082952933</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>0.61477300126040835</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>0.81766717112269349</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>0.69863532184800636</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="7">
         <v>0.65282051282051412</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5.3366992312063072E-2</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>0.54149216338172657</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>0.89042094053023735</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>0.76227987453387736</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="7">
         <v>0.6509401709401722</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>1.873817422860383E-2</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>0.43014313111550168</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>0.96872372624852809</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>0.89582525614717368</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="7">
         <v>0.66004273504273636</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>6.579332246575682E-3</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>0.30297492330530101</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>0.99237710890645126</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>1.14312596600358</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="7">
         <v>0.64846153846153987</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>2.3101297000831579E-3</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>0.1966289050153239</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>0.99260131158567333</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>1.5470126488770339</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="7">
         <v>0.63132478632478772</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>8.1113083078968723E-4</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>0.12940186221950681</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>0.99282551426489529</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>2.140343551147986</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="7">
         <v>0.61495726495726655</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
         <v>2.8480358684358022E-4</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <v>9.3171959422529677E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>0.99265736225547885</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>2.9549844243445991</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <v>0.60239316239316409</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
         <v>1E-4</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>7.4616100845289801E-2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
         <v>0.99265736225547885</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="9">
         <v>4.0002560206929756</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <v>0.59611111111111281</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="67" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="68"/>
+      <c r="C3" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="69" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="30"/>
+      <c r="G16" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" s="32" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="6:13" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="6:13" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="70"/>
+      <c r="G18" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="6:13" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F19" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="6:13" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="F20" s="69" t="s">
+        <v>207</v>
+      </c>
+      <c r="G20" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="H20" s="72" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="6:13" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="71"/>
+      <c r="G21" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="H21" s="73"/>
+    </row>
+    <row r="22" spans="6:13" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="F22" s="71"/>
+      <c r="G22" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="H22" s="73"/>
+    </row>
+    <row r="23" spans="6:13" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="F23" s="71"/>
+      <c r="G23" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="H23" s="73"/>
+    </row>
+    <row r="24" spans="6:13" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="70"/>
+      <c r="G24" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H24" s="74"/>
+    </row>
+    <row r="28" spans="6:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="6:13" ht="57.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="J29" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="K29" s="75"/>
+      <c r="L29" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="M29" s="52"/>
+    </row>
+    <row r="30" spans="6:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="53"/>
+    </row>
+    <row r="31" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="J31" s="42"/>
+      <c r="L31" s="54"/>
+    </row>
+    <row r="32" spans="6:13" x14ac:dyDescent="0.3">
+      <c r="J32" s="29"/>
+      <c r="L32" s="54"/>
+    </row>
+    <row r="33" spans="14:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="14:16" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N34" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="O34" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="P34" s="58" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="14:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N35" s="56"/>
+      <c r="O35" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="P35" s="59"/>
+    </row>
+    <row r="36" spans="14:16" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N36" s="57"/>
+      <c r="O36" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="P36" s="60"/>
+    </row>
+    <row r="37" spans="14:16" ht="46.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N37" s="64" t="s">
+        <v>224</v>
+      </c>
+      <c r="O37" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="P37" s="61" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="14:16" ht="80.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N38" s="65"/>
+      <c r="O38" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="P38" s="62"/>
+    </row>
+    <row r="39" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N39" s="65"/>
+      <c r="O39" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="P39" s="62"/>
+    </row>
+    <row r="40" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N40" s="65"/>
+      <c r="O40" s="49" t="s">
+        <v>229</v>
+      </c>
+      <c r="P40" s="62"/>
+    </row>
+    <row r="41" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N41" s="65"/>
+      <c r="O41" s="49" t="s">
+        <v>227</v>
+      </c>
+      <c r="P41" s="62"/>
+    </row>
+    <row r="42" spans="14:16" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N42" s="66"/>
+      <c r="O42" s="50" t="s">
+        <v>228</v>
+      </c>
+      <c r="P42" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="P34:P36"/>
+    <mergeCell ref="P37:P42"/>
+    <mergeCell ref="N37:N42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>